<commit_message>
add typeRef check and adjust tests
</commit_message>
<xml_diff>
--- a/converter/test/example.xlsx
+++ b/converter/test/example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\excel-to-dmn-plugin\converter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\excel-to-dmn-plugin\converter\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1913661-C6BF-435A-9A8A-C54899D123BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC15A73B-DCC3-4DD8-807C-9326E67EC879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>amount</t>
   </si>
@@ -40,22 +40,19 @@
     <t>&gt; 800</t>
   </si>
   <si>
-    <t>Travel Expenses</t>
-  </si>
-  <si>
     <t>sales</t>
   </si>
   <si>
     <t>&gt; 500</t>
   </si>
   <si>
-    <t>Foo</t>
-  </si>
-  <si>
     <t>management</t>
   </si>
   <si>
     <t>anno1</t>
+  </si>
+  <si>
+    <t>amount &lt; b</t>
   </si>
 </sst>
 </file>
@@ -318,7 +315,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -338,6 +335,9 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -346,25 +346,25 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.5678700000000001</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>